<commit_message>
To Run test tabou all
</commit_message>
<xml_diff>
--- a/olddata/tai12a.txtIter10.xlsx
+++ b/olddata/tai12a.txtIter10.xlsx
@@ -370,13 +370,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>258536</v>
+        <v>251442</v>
       </c>
       <c r="C2">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D2">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -384,13 +384,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C3">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D3">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -398,13 +398,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C4">
-        <v>256370</v>
+        <v>271234</v>
       </c>
       <c r="D4">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -412,13 +412,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C5">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D5">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -426,13 +426,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C6">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D6">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -440,13 +440,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C7">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D7">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -454,13 +454,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C8">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D8">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -468,13 +468,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C9">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D9">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -482,13 +482,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C10">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D10">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -496,13 +496,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C11">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D11">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -510,13 +510,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C12">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D12">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -524,13 +524,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C13">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D13">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -538,13 +538,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C14">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D14">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -552,13 +552,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C15">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D15">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -566,13 +566,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C16">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D16">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -580,13 +580,13 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C17">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D17">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -594,13 +594,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C18">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D18">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -608,13 +608,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C19">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D19">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -622,13 +622,13 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C20">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D20">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -636,13 +636,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C21">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D21">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -650,13 +650,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>253724</v>
+        <v>248232</v>
       </c>
       <c r="C22">
-        <v>256370</v>
+        <v>275600</v>
       </c>
       <c r="D22">
-        <v>339684</v>
+        <v>272396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>